<commit_message>
Update text file for sending and sent messages
</commit_message>
<xml_diff>
--- a/Assets/Editor/StringFile.xlsx
+++ b/Assets/Editor/StringFile.xlsx
@@ -662,24 +662,12 @@
     <t>Cases Closed Negatively</t>
   </si>
   <si>
-    <t>Sending Feedback</t>
-  </si>
-  <si>
-    <t>BASIC_TEXT_FEEDBACK_SENT</t>
-  </si>
-  <si>
-    <t>Feedback Sent</t>
-  </si>
-  <si>
     <t>BASIC_TEXT_ERROR</t>
   </si>
   <si>
     <t>Error</t>
   </si>
   <si>
-    <t>BASIC_TEXT_SENDING_FEEDBACK</t>
-  </si>
-  <si>
     <t>Καλώς ήρθατε στο παιχνίδι διαχείρισης αστυνομικών πόρων. Θα αναλάβετε συντονιστικό ρόλο στην διάθεση αστυνομικών για την επίλυση προβλημάτων της πόλης. Χρησιμοποιήστε τη δύναμη των διαθέσιμων αστυνομικών σε συνδυασμό με τις πληροφορίες από τους πολίτες για να κρατήσετε την πόλη ασφαλή και τους πολίτες ευχαριστημένους. Εφιστούμε την προσοχή σας καθώς η δύναμη των διαθέσιμων αστυνομικών είναι περιορισμένη και οι πολίτες δεν αναφέρουν πάντα με ακρίβεια τα συμβάντα</t>
   </si>
   <si>
@@ -1455,6 +1443,18 @@
   </si>
   <si>
     <t>Enter email to get regular INSPEC2T Updates</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_SENDING</t>
+  </si>
+  <si>
+    <t>Sending</t>
+  </si>
+  <si>
+    <t>Sent</t>
+  </si>
+  <si>
+    <t>BASIC_TEXT_SENT</t>
   </si>
 </sst>
 </file>
@@ -1852,8 +1852,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1891,13 +1891,13 @@
         <v>204</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1925,10 +1925,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>123</v>
@@ -1948,7 +1948,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1959,13 +1959,13 @@
         <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1976,13 +1976,13 @@
         <v>116</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1993,10 +1993,10 @@
         <v>63</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>124</v>
@@ -2010,13 +2010,13 @@
         <v>51</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2027,13 +2027,13 @@
         <v>50</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2044,13 +2044,13 @@
         <v>61</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2061,10 +2061,10 @@
         <v>80</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>125</v>
@@ -2078,13 +2078,13 @@
         <v>40</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2095,13 +2095,13 @@
         <v>97</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2112,10 +2112,10 @@
         <v>20</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>126</v>
@@ -2129,13 +2129,13 @@
         <v>21</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2146,10 +2146,10 @@
         <v>22</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>127</v>
@@ -2163,10 +2163,10 @@
         <v>23</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>128</v>
@@ -2180,10 +2180,10 @@
         <v>25</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>129</v>
@@ -2197,13 +2197,13 @@
         <v>34</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2214,13 +2214,13 @@
         <v>27</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2231,10 +2231,10 @@
         <v>29</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>130</v>
@@ -2248,13 +2248,13 @@
         <v>31</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2268,10 +2268,10 @@
         <v>47</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -2279,16 +2279,16 @@
         <v>41</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2299,10 +2299,10 @@
         <v>37</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>131</v>
@@ -2316,13 +2316,13 @@
         <v>132</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2333,13 +2333,13 @@
         <v>43</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2350,13 +2350,13 @@
         <v>49</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2367,10 +2367,10 @@
         <v>60</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>133</v>
@@ -2387,7 +2387,7 @@
         <v>155</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>166</v>
@@ -2401,10 +2401,10 @@
         <v>86</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>134</v>
@@ -2418,10 +2418,10 @@
         <v>206</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>207</v>
@@ -2435,13 +2435,13 @@
         <v>209</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2452,13 +2452,13 @@
         <v>211</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2469,13 +2469,13 @@
         <v>85</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2489,7 +2489,7 @@
         <v>57</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>135</v>
@@ -2506,7 +2506,7 @@
         <v>59</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>136</v>
@@ -2520,10 +2520,10 @@
         <v>53</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>137</v>
@@ -2537,13 +2537,13 @@
         <v>84</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2554,10 +2554,10 @@
         <v>54</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>138</v>
@@ -2571,13 +2571,13 @@
         <v>150</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2588,13 +2588,13 @@
         <v>92</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2605,13 +2605,13 @@
         <v>93</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2622,13 +2622,13 @@
         <v>91</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2639,10 +2639,10 @@
         <v>99</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>139</v>
@@ -2659,7 +2659,7 @@
         <v>101</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>140</v>
@@ -2673,13 +2673,13 @@
         <v>103</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2690,10 +2690,10 @@
         <v>152</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>165</v>
@@ -2707,10 +2707,10 @@
         <v>186</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E50" s="10" t="s">
         <v>187</v>
@@ -2724,13 +2724,13 @@
         <v>177</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2741,13 +2741,13 @@
         <v>180</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2758,13 +2758,13 @@
         <v>178</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2775,13 +2775,13 @@
         <v>181</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2792,13 +2792,13 @@
         <v>179</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2809,10 +2809,10 @@
         <v>183</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>184</v>
@@ -2826,13 +2826,13 @@
         <v>205</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2843,13 +2843,13 @@
         <v>189</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2860,13 +2860,13 @@
         <v>82</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2877,13 +2877,13 @@
         <v>95</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2894,13 +2894,13 @@
         <v>105</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2911,13 +2911,13 @@
         <v>65</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2928,13 +2928,13 @@
         <v>67</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -2945,13 +2945,13 @@
         <v>69</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -2962,13 +2962,13 @@
         <v>78</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2979,13 +2979,13 @@
         <v>72</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2996,13 +2996,13 @@
         <v>77</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3013,13 +3013,13 @@
         <v>202</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
@@ -3027,16 +3027,16 @@
         <v>147</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
@@ -3044,16 +3044,16 @@
         <v>148</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3061,16 +3061,16 @@
         <v>149</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3081,13 +3081,13 @@
         <v>75</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3098,13 +3098,13 @@
         <v>109</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3115,13 +3115,13 @@
         <v>108</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3132,10 +3132,10 @@
         <v>37</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E75" s="7" t="s">
         <v>131</v>
@@ -3149,10 +3149,10 @@
         <v>112</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>164</v>
@@ -3163,16 +3163,16 @@
         <v>113</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3180,16 +3180,16 @@
         <v>114</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3200,10 +3200,10 @@
         <v>145</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E79" s="7" t="s">
         <v>146</v>
@@ -3217,13 +3217,13 @@
         <v>168</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3268,10 +3268,10 @@
         <v>143</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>163</v>
@@ -3285,13 +3285,13 @@
         <v>144</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3299,16 +3299,16 @@
         <v>156</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3316,16 +3316,16 @@
         <v>157</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3333,16 +3333,16 @@
         <v>160</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3350,16 +3350,16 @@
         <v>158</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3367,16 +3367,16 @@
         <v>159</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3384,16 +3384,16 @@
         <v>161</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3401,16 +3401,16 @@
         <v>162</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3424,10 +3424,10 @@
         <v>203</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E92" s="10" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3438,10 +3438,10 @@
         <v>194</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E93" s="10" t="s">
         <v>197</v>
@@ -3455,10 +3455,10 @@
         <v>25</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>129</v>
@@ -3472,10 +3472,10 @@
         <v>195</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E95" s="10" t="s">
         <v>198</v>
@@ -3489,10 +3489,10 @@
         <v>196</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>199</v>
@@ -3506,21 +3506,21 @@
         <v>201</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="4" t="s">
-        <v>217</v>
+        <v>473</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>212</v>
+        <v>474</v>
       </c>
       <c r="C98" s="12" t="s">
         <v>0</v>
@@ -3534,10 +3534,10 @@
     </row>
     <row r="99" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="4" t="s">
-        <v>213</v>
+        <v>476</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>214</v>
+        <v>475</v>
       </c>
       <c r="C99" s="12" t="s">
         <v>0</v>
@@ -3551,10 +3551,10 @@
     </row>
     <row r="100" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C100" s="12" t="s">
         <v>0</v>
@@ -3568,10 +3568,10 @@
     </row>
     <row r="101" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="4" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="C101" s="12" t="s">
         <v>0</v>
@@ -3585,10 +3585,10 @@
     </row>
     <row r="102" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="4" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C102" s="12" t="s">
         <v>0</v>
@@ -3602,10 +3602,10 @@
     </row>
     <row r="103" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="4" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C103" s="12" t="s">
         <v>0</v>
@@ -3619,10 +3619,10 @@
     </row>
     <row r="104" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="4" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C104" s="12" t="s">
         <v>0</v>
@@ -3636,10 +3636,10 @@
     </row>
     <row r="105" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="4" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C105" s="12" t="s">
         <v>0</v>
@@ -3653,10 +3653,10 @@
     </row>
     <row r="106" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="4" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C106" s="12" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
make description easier to understand Add new logo that has resource force in the icon
</commit_message>
<xml_diff>
--- a/Assets/Editor/StringFile.xlsx
+++ b/Assets/Editor/StringFile.xlsx
@@ -638,9 +638,6 @@
     <t>Oplossing</t>
   </si>
   <si>
-    <t>Welcome to resource force, take on the role of a police operator and help to solve crimes across the city. Utilise the power of dispatch officers along with information from citizens to keep the city safe and the citizens happy! Be careful, you only have a limited number of officers and citizens may not always provide good information</t>
-  </si>
-  <si>
     <t>End Turn Summary</t>
   </si>
   <si>
@@ -1455,6 +1452,9 @@
   </si>
   <si>
     <t>BASIC_TEXT_SENT</t>
+  </si>
+  <si>
+    <t>Take on the role of a police operator and help to solve crimes across the city.\n\nKeep the city safe and citizens happy with the power of dispatch officers along with information from citizens.\n\nBut be careful, you only have a limited number of officers and citizens may not always provide good information</t>
   </si>
 </sst>
 </file>
@@ -1852,8 +1852,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1888,16 +1888,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>204</v>
+        <v>476</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1925,10 +1925,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>123</v>
@@ -1948,7 +1948,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1959,13 +1959,13 @@
         <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1976,13 +1976,13 @@
         <v>116</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1993,10 +1993,10 @@
         <v>63</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>124</v>
@@ -2010,13 +2010,13 @@
         <v>51</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2027,13 +2027,13 @@
         <v>50</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2044,13 +2044,13 @@
         <v>61</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2061,10 +2061,10 @@
         <v>80</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>125</v>
@@ -2078,13 +2078,13 @@
         <v>40</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2095,13 +2095,13 @@
         <v>97</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2112,10 +2112,10 @@
         <v>20</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>126</v>
@@ -2129,13 +2129,13 @@
         <v>21</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2146,10 +2146,10 @@
         <v>22</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>127</v>
@@ -2163,10 +2163,10 @@
         <v>23</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>128</v>
@@ -2180,10 +2180,10 @@
         <v>25</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>129</v>
@@ -2197,13 +2197,13 @@
         <v>34</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2214,13 +2214,13 @@
         <v>27</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2231,10 +2231,10 @@
         <v>29</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>130</v>
@@ -2248,13 +2248,13 @@
         <v>31</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2268,10 +2268,10 @@
         <v>47</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -2279,16 +2279,16 @@
         <v>41</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>457</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="9" t="s">
         <v>459</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2299,10 +2299,10 @@
         <v>37</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>131</v>
@@ -2316,13 +2316,13 @@
         <v>132</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2333,13 +2333,13 @@
         <v>43</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2350,13 +2350,13 @@
         <v>49</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2367,10 +2367,10 @@
         <v>60</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>133</v>
@@ -2387,7 +2387,7 @@
         <v>155</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>166</v>
@@ -2401,10 +2401,10 @@
         <v>86</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>134</v>
@@ -2415,50 +2415,50 @@
         <v>153</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E33" s="10" t="s">
         <v>206</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>209</v>
-      </c>
       <c r="C34" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>211</v>
-      </c>
       <c r="C35" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2469,13 +2469,13 @@
         <v>85</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2489,7 +2489,7 @@
         <v>57</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>135</v>
@@ -2506,7 +2506,7 @@
         <v>59</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>136</v>
@@ -2520,10 +2520,10 @@
         <v>53</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>137</v>
@@ -2537,13 +2537,13 @@
         <v>84</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2554,10 +2554,10 @@
         <v>54</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>138</v>
@@ -2571,13 +2571,13 @@
         <v>150</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2588,13 +2588,13 @@
         <v>92</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2605,13 +2605,13 @@
         <v>93</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2622,13 +2622,13 @@
         <v>91</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2639,10 +2639,10 @@
         <v>99</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>139</v>
@@ -2659,7 +2659,7 @@
         <v>101</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>140</v>
@@ -2673,13 +2673,13 @@
         <v>103</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2690,10 +2690,10 @@
         <v>152</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>165</v>
@@ -2707,10 +2707,10 @@
         <v>186</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E50" s="10" t="s">
         <v>187</v>
@@ -2724,13 +2724,13 @@
         <v>177</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2741,13 +2741,13 @@
         <v>180</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2758,13 +2758,13 @@
         <v>178</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2775,13 +2775,13 @@
         <v>181</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2792,13 +2792,13 @@
         <v>179</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2809,10 +2809,10 @@
         <v>183</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>184</v>
@@ -2823,16 +2823,16 @@
         <v>185</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2843,13 +2843,13 @@
         <v>189</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2860,13 +2860,13 @@
         <v>82</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2877,13 +2877,13 @@
         <v>95</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2894,13 +2894,13 @@
         <v>105</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2911,13 +2911,13 @@
         <v>65</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2928,13 +2928,13 @@
         <v>67</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -2945,13 +2945,13 @@
         <v>69</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -2962,13 +2962,13 @@
         <v>78</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2979,13 +2979,13 @@
         <v>72</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2996,13 +2996,13 @@
         <v>77</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3013,13 +3013,13 @@
         <v>202</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
@@ -3027,16 +3027,16 @@
         <v>147</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
@@ -3044,16 +3044,16 @@
         <v>148</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="C70" s="8" t="s">
         <v>449</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="D70" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="E70" s="9" t="s">
         <v>451</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3061,16 +3061,16 @@
         <v>149</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3081,13 +3081,13 @@
         <v>75</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3098,13 +3098,13 @@
         <v>109</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3115,13 +3115,13 @@
         <v>108</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3132,10 +3132,10 @@
         <v>37</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E75" s="7" t="s">
         <v>131</v>
@@ -3149,10 +3149,10 @@
         <v>112</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>164</v>
@@ -3163,16 +3163,16 @@
         <v>113</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C77" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="E77" s="7" t="s">
         <v>442</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3180,16 +3180,16 @@
         <v>114</v>
       </c>
       <c r="B78" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="D78" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="C78" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="D78" s="5" t="s">
+      <c r="E78" s="7" t="s">
         <v>439</v>
-      </c>
-      <c r="E78" s="7" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3200,10 +3200,10 @@
         <v>145</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E79" s="7" t="s">
         <v>146</v>
@@ -3217,13 +3217,13 @@
         <v>168</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3268,10 +3268,10 @@
         <v>143</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>163</v>
@@ -3285,13 +3285,13 @@
         <v>144</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3299,16 +3299,16 @@
         <v>156</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3316,16 +3316,16 @@
         <v>157</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C86" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="E86" s="8" t="s">
         <v>432</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="E86" s="8" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3333,16 +3333,16 @@
         <v>160</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3350,16 +3350,16 @@
         <v>158</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C88" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="D88" s="5" t="s">
         <v>426</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="E88" s="8" t="s">
         <v>427</v>
-      </c>
-      <c r="E88" s="8" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3367,16 +3367,16 @@
         <v>159</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3384,16 +3384,16 @@
         <v>161</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3401,16 +3401,16 @@
         <v>162</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C91" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D91" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="E91" s="8" t="s">
         <v>419</v>
-      </c>
-      <c r="E91" s="8" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3424,10 +3424,10 @@
         <v>203</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E92" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3438,10 +3438,10 @@
         <v>194</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E93" s="10" t="s">
         <v>197</v>
@@ -3455,10 +3455,10 @@
         <v>25</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>129</v>
@@ -3472,10 +3472,10 @@
         <v>195</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E95" s="10" t="s">
         <v>198</v>
@@ -3489,10 +3489,10 @@
         <v>196</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>199</v>
@@ -3506,21 +3506,21 @@
         <v>201</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="B98" s="5" t="s">
         <v>473</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>474</v>
       </c>
       <c r="C98" s="12" t="s">
         <v>0</v>
@@ -3534,10 +3534,10 @@
     </row>
     <row r="99" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C99" s="12" t="s">
         <v>0</v>
@@ -3551,10 +3551,10 @@
     </row>
     <row r="100" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B100" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>213</v>
       </c>
       <c r="C100" s="12" t="s">
         <v>0</v>
@@ -3568,10 +3568,10 @@
     </row>
     <row r="101" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="B101" s="5" t="s">
         <v>461</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>462</v>
       </c>
       <c r="C101" s="12" t="s">
         <v>0</v>
@@ -3585,10 +3585,10 @@
     </row>
     <row r="102" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C102" s="12" t="s">
         <v>0</v>
@@ -3602,10 +3602,10 @@
     </row>
     <row r="103" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="B103" s="5" t="s">
         <v>465</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>466</v>
       </c>
       <c r="C103" s="12" t="s">
         <v>0</v>
@@ -3619,10 +3619,10 @@
     </row>
     <row r="104" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="B104" s="5" t="s">
         <v>467</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>468</v>
       </c>
       <c r="C104" s="12" t="s">
         <v>0</v>
@@ -3636,10 +3636,10 @@
     </row>
     <row r="105" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>469</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>470</v>
       </c>
       <c r="C105" s="12" t="s">
         <v>0</v>
@@ -3653,10 +3653,10 @@
     </row>
     <row r="106" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="B106" s="5" t="s">
         <v>471</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>472</v>
       </c>
       <c r="C106" s="12" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Dont try to laod new content when selecting a new location
</commit_message>
<xml_diff>
--- a/Assets/Editor/StringFile.xlsx
+++ b/Assets/Editor/StringFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="486">
   <si>
     <t>XXXX</t>
   </si>
@@ -1455,13 +1455,40 @@
   </si>
   <si>
     <t>Take on the role of a police operator and help to solve crimes across the city.\n\nKeep the city safe and citizens happy with the power of dispatch officers along with information from citizens.\n\nBut be careful, you only have a limited number of officers and citizens may not always provide good information</t>
+  </si>
+  <si>
+    <t>Versturen</t>
+  </si>
+  <si>
+    <t>Verstuurd</t>
+  </si>
+  <si>
+    <t>Fout opgetreden</t>
+  </si>
+  <si>
+    <t>Content ophalen...</t>
+  </si>
+  <si>
+    <t>Controleren op nieuwe content...</t>
+  </si>
+  <si>
+    <t>Nieuwe content gevonden</t>
+  </si>
+  <si>
+    <t>Geen nieuwe content gevonden</t>
+  </si>
+  <si>
+    <t>Optioneel</t>
+  </si>
+  <si>
+    <t>Voer e-mail in om INSPEC2T updates te ontvangen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1483,8 +1510,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1499,6 +1532,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1564,7 +1603,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1852,8 +1891,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98:C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3523,7 +3562,7 @@
         <v>473</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>0</v>
+        <v>477</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>0</v>
@@ -3540,7 +3579,7 @@
         <v>474</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>0</v>
+        <v>478</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>0</v>
@@ -3557,7 +3596,7 @@
         <v>212</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>0</v>
+        <v>479</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>0</v>
@@ -3574,7 +3613,7 @@
         <v>461</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>0</v>
@@ -3591,7 +3630,7 @@
         <v>462</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>0</v>
+        <v>481</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>0</v>
@@ -3608,7 +3647,7 @@
         <v>465</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>0</v>
+        <v>482</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>0</v>
@@ -3625,7 +3664,7 @@
         <v>467</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>0</v>
+        <v>483</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>0</v>
@@ -3642,7 +3681,7 @@
         <v>469</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>0</v>
+        <v>484</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>0</v>
@@ -3659,7 +3698,7 @@
         <v>471</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>0</v>
+        <v>485</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>0</v>

</xml_diff>